<commit_message>
Desarrollo de la teoría musical Replay - IYAZ es la canción de prueba , no se colocó el lector de canciones en index todavía
</commit_message>
<xml_diff>
--- a/Cancionero Vigil (Alpha).xlsx
+++ b/Cancionero Vigil (Alpha).xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PortableApps\smartgit-portable\Git_Proyectos\Canciones Vigil\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397865DF-2608-4866-AA5E-EB97AA7ADE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Index" sheetId="1" r:id="rId1"/>
+    <sheet name="Replay(prueba)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +25,68 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+  <si>
+    <t>Verso</t>
+  </si>
+  <si>
+    <t>Acorde</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>N° Tiempo</t>
+  </si>
+  <si>
+    <t>Partes de Compas:</t>
+  </si>
+  <si>
+    <t>COMPAS</t>
+  </si>
+  <si>
+    <t>1 Tiempo</t>
+  </si>
+  <si>
+    <t>2 Tiempo</t>
+  </si>
+  <si>
+    <t>3 Tiempo</t>
+  </si>
+  <si>
+    <t>4 Tiempo</t>
+  </si>
+  <si>
+    <t>Acordes</t>
+  </si>
+  <si>
+    <t>Parte del verso…</t>
+  </si>
+  <si>
+    <t>N° Compas</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Shawtys like a melo</t>
+  </si>
+  <si>
+    <t>dy in my head</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +94,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,18 +165,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -330,13 +495,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2CD92-9487-4DC1-8D1C-E88C0F5EF3CB}">
+  <dimension ref="C2:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="51" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Primer párrafo hecho, falta configurar el index
</commit_message>
<xml_diff>
--- a/Cancionero Vigil (Alpha).xlsx
+++ b/Cancionero Vigil (Alpha).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PortableApps\smartgit-portable\Git_Proyectos\Canciones Vigil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397865DF-2608-4866-AA5E-EB97AA7ADE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09570171-A39C-4335-97A1-90F51105D3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Verso</t>
   </si>
@@ -79,7 +79,25 @@
     <t>Shawtys like a melo</t>
   </si>
   <si>
-    <t>dy in my head</t>
+    <t xml:space="preserve">dy in my head that i </t>
+  </si>
+  <si>
+    <t>cant keep out</t>
+  </si>
+  <si>
+    <t>got me singing like</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na ra na na </t>
+  </si>
+  <si>
+    <t>every day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Its like my ipod </t>
+  </si>
+  <si>
+    <t>stuck-on replay</t>
   </si>
 </sst>
 </file>
@@ -516,10 +534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2CD92-9487-4DC1-8D1C-E88C0F5EF3CB}">
-  <dimension ref="C2:K8"/>
+  <dimension ref="C2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +599,9 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="H5" s="9" t="s">
         <v>10</v>
       </c>
@@ -600,6 +621,9 @@
       <c r="E6" s="1">
         <v>2</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>11</v>
       </c>
@@ -608,19 +632,87 @@
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comienzo del formato para las fórmulas, no se hizo ninguna fórmula para la búsqueda, existe una fórmula de ejemplo.
</commit_message>
<xml_diff>
--- a/Cancionero Vigil (Alpha).xlsx
+++ b/Cancionero Vigil (Alpha).xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PortableApps\smartgit-portable\Git_Proyectos\Canciones Vigil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09570171-A39C-4335-97A1-90F51105D3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95753183-9DF5-4C6C-98FE-44419E385125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
-    <sheet name="Replay(prueba)" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabla de la cancion" sheetId="3" r:id="rId2"/>
+    <sheet name="OPERACIONES DE FORMULAS" sheetId="5" r:id="rId3"/>
+    <sheet name="CANCIONES" sheetId="2" r:id="rId4"/>
+    <sheet name="Formula de busqueda" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Verso</t>
   </si>
@@ -43,9 +52,6 @@
     <t>Partes de Compas:</t>
   </si>
   <si>
-    <t>COMPAS</t>
-  </si>
-  <si>
     <t>1 Tiempo</t>
   </si>
   <si>
@@ -79,15 +85,6 @@
     <t>Shawtys like a melo</t>
   </si>
   <si>
-    <t xml:space="preserve">dy in my head that i </t>
-  </si>
-  <si>
-    <t>cant keep out</t>
-  </si>
-  <si>
-    <t>got me singing like</t>
-  </si>
-  <si>
     <t xml:space="preserve">na ra na na </t>
   </si>
   <si>
@@ -98,6 +95,69 @@
   </si>
   <si>
     <t>stuck-on replay</t>
+  </si>
+  <si>
+    <t>Cancion:</t>
+  </si>
+  <si>
+    <t>Replay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dy in my </t>
+  </si>
+  <si>
+    <t>head that i cant keep</t>
+  </si>
+  <si>
+    <t>out got me singing like</t>
+  </si>
+  <si>
+    <t>1 COMPAS</t>
+  </si>
+  <si>
+    <t>Cancion</t>
+  </si>
+  <si>
+    <t>Partes del compas</t>
+  </si>
+  <si>
+    <t>Calificacion</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Ariana</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Lucia</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Rubi</t>
+  </si>
+  <si>
+    <t>Juliana</t>
+  </si>
+  <si>
+    <t>Justa</t>
+  </si>
+  <si>
+    <t>Indicio de busqueda:</t>
+  </si>
+  <si>
+    <t>Nombres:</t>
   </si>
 </sst>
 </file>
@@ -175,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -201,20 +261,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -228,6 +300,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -522,32 +607,88 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="str">
+        <f>CANCIONES!E5</f>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4790C0F-4D04-4C01-A157-4DDB9E8A8075}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF2396F-2B00-4C99-BED7-890F3FD75333}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2CD92-9487-4DC1-8D1C-E88C0F5EF3CB}">
-  <dimension ref="C2:K12"/>
+  <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -555,164 +696,218 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H3" s="4" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="7" t="s">
+    </row>
+    <row r="4" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10">
+        <v>4</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="10">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10">
+        <v>3</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F10" s="10">
         <v>3</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="G10" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="10">
+        <v>4</v>
+      </c>
+      <c r="G11" s="10">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="10">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F12" s="10">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10">
         <v>3</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="1">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -725,4 +920,221 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F895926B-BC39-450E-897D-27FFAB8ED0C4}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>13</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="1">
+        <f>IF($A$2:$A$18=$F$2,ROW())</f>
+        <v>2</v>
+      </c>
+      <c r="L2" t="str">
+        <f>INDEX($B$1:$B$10,SMALL($I$2:$I$14,ROW()-1))</f>
+        <v>Ariana</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <f t="shared" ref="I3:I14" si="0">IF($A$2:$A$18=$F$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L13" si="1">INDEX($B$1:$B$10,SMALL($I$2:$I$14,ROW()-1))</f>
+        <v>Lucia</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>Rubi</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>14</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>12</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L8" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se hizo un recopilador de la canción para mostrar la tabla buscada, aun no se ha configurado index, se inserto un ComboBox de búsqueda sin configurar.
</commit_message>
<xml_diff>
--- a/Cancionero Vigil (Alpha).xlsx
+++ b/Cancionero Vigil (Alpha).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PortableApps\smartgit-portable\Git_Proyectos\Canciones Vigil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95753183-9DF5-4C6C-98FE-44419E385125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489679C9-6240-4777-B023-097EA1E4B261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Verso</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Nombres:</t>
+  </si>
+  <si>
+    <t>FILAS DETECTADAS</t>
+  </si>
+  <si>
+    <t>Filas encontradas</t>
   </si>
 </sst>
 </file>
@@ -280,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,6 +315,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -334,6 +346,73 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>19049</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>19051</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>2047874</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>76201</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="ComboBox1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB6FF1B-E1D2-4003-A93D-F965A64F3143}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,11 +677,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,44 +721,1295 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId3" name="ComboBox1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" linkedCell="C2" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>2047875</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId3" name="ComboBox1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4790C0F-4D04-4C01-A157-4DDB9E8A8075}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Hoja2"/>
+  <dimension ref="B1:K73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C2">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Shawtys like a melo</v>
+      </c>
+      <c r="E2" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>E</v>
+      </c>
+      <c r="F2">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C3">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D3" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v xml:space="preserve">dy in my </v>
+      </c>
+      <c r="E3" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>C</v>
+      </c>
+      <c r="F3">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K3" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C4">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D4" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>head that i cant keep</v>
+      </c>
+      <c r="E4" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>G</v>
+      </c>
+      <c r="F4">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C5">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>out got me singing like</v>
+      </c>
+      <c r="E5" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>D</v>
+      </c>
+      <c r="F5">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K5" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C6">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D6" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v xml:space="preserve">na ra na na </v>
+      </c>
+      <c r="E6" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>E</v>
+      </c>
+      <c r="F6">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C7">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D7" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>every day</v>
+      </c>
+      <c r="E7" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>C</v>
+      </c>
+      <c r="F7">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C8">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D8" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v xml:space="preserve">Its like my ipod </v>
+      </c>
+      <c r="E8" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>G</v>
+      </c>
+      <c r="F8">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C9">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D9" t="str">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>stuck-on replay</v>
+      </c>
+      <c r="E9" t="str">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>D</v>
+      </c>
+      <c r="F9">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="10">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C10" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D10" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E10" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F10" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G10" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K10" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C11" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D11" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E11" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F11" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G11" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K11" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C12" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D12" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E12" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F12" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G12" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K12" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C13" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D13" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E13" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F13" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G13" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K13" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C14" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D14" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E14" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F14" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G14" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K14" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C15" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D15" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E15" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F15" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G15" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K15" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C16" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D16" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E16" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F16" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G16" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K16" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C17" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D17" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E17" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F17" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G17" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K17" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C18" t="e">
+        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D18" t="e">
+        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E18" t="e">
+        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F18" t="e">
+        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G18" t="e">
+        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K18" s="10" t="e">
+        <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF2396F-2B00-4C99-BED7-890F3FD75333}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Hoja3"/>
+  <dimension ref="D4:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2CD92-9487-4DC1-8D1C-E88C0F5EF3CB}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,30 +2042,30 @@
       </c>
     </row>
     <row r="4" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
@@ -924,6 +2255,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F895926B-BC39-450E-897D-27FFAB8ED0C4}">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
El buscador esta en desarrollo, con la ayuda de una fórmula y un control ActiveX
</commit_message>
<xml_diff>
--- a/Cancionero Vigil (Alpha).xlsx
+++ b/Cancionero Vigil (Alpha).xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PortableApps\smartgit-portable\Git_Proyectos\Canciones Vigil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489679C9-6240-4777-B023-097EA1E4B261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A3D565-65DB-47BE-97FE-7C031DF68F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Verso</t>
   </si>
@@ -164,13 +164,16 @@
   </si>
   <si>
     <t>Filas encontradas</t>
+  </si>
+  <si>
+    <t>Buscador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +186,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -286,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,16 +368,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>19049</xdr:colOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>771524</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>19051</xdr:rowOff>
+          <xdr:rowOff>28576</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>2047874</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>809624</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>76201</xdr:rowOff>
+          <xdr:rowOff>85726</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -682,7 +692,7 @@
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +719,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="str">
-        <f>CANCIONES!E5</f>
+        <f>CANCIONES!F5</f>
         <v>E</v>
       </c>
     </row>
@@ -727,19 +737,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="1025" r:id="rId3" name="ComboBox1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" linkedCell="C2" r:id="rId4">
+          <controlPr defaultSize="0" autoLine="0" linkedCell="C2" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
                 <xdr:row>1</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>2047875</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>809625</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -793,243 +803,243 @@
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C2" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D2" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D2" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Shawtys like a melo</v>
-      </c>
-      <c r="E2" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E2" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>E</v>
-      </c>
-      <c r="F2">
+        <v>#NUM!</v>
+      </c>
+      <c r="F2" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>1</v>
-      </c>
-      <c r="G2">
+        <v>#NUM!</v>
+      </c>
+      <c r="G2" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K2" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>5</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C3" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D3" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D3" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v xml:space="preserve">dy in my </v>
-      </c>
-      <c r="E3" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E3" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>C</v>
-      </c>
-      <c r="F3">
+        <v>#NUM!</v>
+      </c>
+      <c r="F3" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>1</v>
-      </c>
-      <c r="G3">
+        <v>#NUM!</v>
+      </c>
+      <c r="G3" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>3</v>
-      </c>
-      <c r="K3" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K3" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>6</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C4" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D4" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D4" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>head that i cant keep</v>
-      </c>
-      <c r="E4" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E4" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>G</v>
-      </c>
-      <c r="F4">
+        <v>#NUM!</v>
+      </c>
+      <c r="F4" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>2</v>
-      </c>
-      <c r="G4">
+        <v>#NUM!</v>
+      </c>
+      <c r="G4" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K4" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>7</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C5" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D5" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D5" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>out got me singing like</v>
-      </c>
-      <c r="E5" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E5" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>D</v>
-      </c>
-      <c r="F5">
+        <v>#NUM!</v>
+      </c>
+      <c r="F5" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>2</v>
-      </c>
-      <c r="G5">
+        <v>#NUM!</v>
+      </c>
+      <c r="G5" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>3</v>
-      </c>
-      <c r="K5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K5" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>8</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C6">
+      <c r="B6" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C6" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D6" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D6" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v xml:space="preserve">na ra na na </v>
-      </c>
-      <c r="E6" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E6" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>E</v>
-      </c>
-      <c r="F6">
+        <v>#NUM!</v>
+      </c>
+      <c r="F6" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>3</v>
-      </c>
-      <c r="G6">
+        <v>#NUM!</v>
+      </c>
+      <c r="G6" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K6" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>9</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C7">
+      <c r="B7" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C7" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D7" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D7" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>every day</v>
-      </c>
-      <c r="E7" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E7" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>C</v>
-      </c>
-      <c r="F7">
+        <v>#NUM!</v>
+      </c>
+      <c r="F7" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>3</v>
-      </c>
-      <c r="G7">
+        <v>#NUM!</v>
+      </c>
+      <c r="G7" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>3</v>
-      </c>
-      <c r="K7" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K7" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>10</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C8">
+      <c r="B8" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C8" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D8" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D8" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v xml:space="preserve">Its like my ipod </v>
-      </c>
-      <c r="E8" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E8" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>G</v>
-      </c>
-      <c r="F8">
+        <v>#NUM!</v>
+      </c>
+      <c r="F8" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="G8">
+        <v>#NUM!</v>
+      </c>
+      <c r="G8" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K8" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>11</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="str">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>Replay</v>
-      </c>
-      <c r="C9">
+      <c r="B9" t="e">
+        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C9" t="e">
         <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="D9" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D9" t="e">
         <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>stuck-on replay</v>
-      </c>
-      <c r="E9" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="E9" t="e">
         <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>D</v>
-      </c>
-      <c r="F9">
+        <v>#NUM!</v>
+      </c>
+      <c r="F9" t="e">
         <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>4</v>
-      </c>
-      <c r="G9">
+        <v>#NUM!</v>
+      </c>
+      <c r="G9" t="e">
         <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>3</v>
-      </c>
-      <c r="K9" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K9" s="10" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>12</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -1657,51 +1667,51 @@
       </c>
     </row>
     <row r="5" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>5</v>
+      <c r="D5" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>6</v>
+      <c r="D6" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>7</v>
+      <c r="D7" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>8</v>
+      <c r="D8" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D9">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>9</v>
+      <c r="D9" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>10</v>
+      <c r="D10" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>11</v>
+      <c r="D11" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>12</v>
+      <c r="D12" t="b">
+        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="4:4" x14ac:dyDescent="0.25">
@@ -2006,10 +2016,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2CD92-9487-4DC1-8D1C-E88C0F5EF3CB}">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="B2:K12"/>
+  <dimension ref="A2:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,237 +2029,264 @@
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>0</v>
-      </c>
       <c r="E4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="I4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
+        <f>IF(B5=1,COUNTIF($B$5:B5,1),"")</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="17">
+        <f>--ISNUMBER(IFERROR(SEARCH(Index!$C$2,C5,1),""))</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10">
+      <c r="D5" s="10">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>2</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="8"/>
+      <c r="K5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10">
+      <c r="D6" s="10">
         <v>4</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10">
+      <c r="G6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="10">
         <v>3</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="10">
+      <c r="D7" s="10">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="10">
+      <c r="G7" s="10">
         <v>2</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="10">
+      <c r="D8" s="10">
         <v>4</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="10">
+      <c r="G8" s="10">
         <v>2</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10">
+      <c r="D9" s="10">
         <v>4</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="G9" s="10">
         <v>3</v>
       </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10">
+      <c r="D10" s="10">
         <v>4</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="F10" s="10">
-        <v>3</v>
       </c>
       <c r="G10" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="H10" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10">
+      <c r="D11" s="10">
         <v>4</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="10">
+      <c r="G11" s="10">
         <v>4</v>
       </c>
-      <c r="G11" s="10">
+      <c r="H11" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="10">
+      <c r="D12" s="10">
         <v>4</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="10">
+      <c r="G12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="10">
+      <c r="H12" s="10">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:L6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Esta es la versión alpha sin código
</commit_message>
<xml_diff>
--- a/Cancionero Vigil (Alpha).xlsx
+++ b/Cancionero Vigil (Alpha).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PortableApps\smartgit-portable\Git_Proyectos\Canciones Vigil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A3D565-65DB-47BE-97FE-7C031DF68F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30958C6E-A18D-4083-B8DC-5C2DE48216F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Verso</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>Buscador</t>
+  </si>
+  <si>
+    <t>Prioridad del buscador</t>
+  </si>
+  <si>
+    <t>CANCIONES DETECTADAS</t>
+  </si>
+  <si>
+    <t>Otra cancion</t>
   </si>
 </sst>
 </file>
@@ -250,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -291,11 +300,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,6 +327,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,26 +355,13 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,15 +395,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>771524</xdr:colOff>
+          <xdr:colOff>771525</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>28576</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>809624</xdr:colOff>
+          <xdr:colOff>809625</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>85726</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -387,7 +413,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB6FF1B-E1D2-4003-A93D-F965A64F3143}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -691,8 +717,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +795,7 @@
   <dimension ref="B1:K73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,559 +806,639 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C2" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D2" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F2" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G2" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K2" s="10" t="e">
+      <c r="B2" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C2">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Shawtys like a melo</v>
+      </c>
+      <c r="E2" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>E</v>
+      </c>
+      <c r="F2">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C3" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D3" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E3" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F3" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G3" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K3" s="10" t="e">
+      <c r="B3" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C3">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D3" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v xml:space="preserve">dy in my </v>
+      </c>
+      <c r="E3" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>C</v>
+      </c>
+      <c r="F3">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K3" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C4" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D4" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E4" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F4" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G4" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K4" s="10" t="e">
+      <c r="B4" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C4">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D4" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>head that i cant keep</v>
+      </c>
+      <c r="E4" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>G</v>
+      </c>
+      <c r="F4">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C5" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D5" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E5" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G5" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K5" s="10" t="e">
+      <c r="B5" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C5">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D5" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>out got me singing like</v>
+      </c>
+      <c r="E5" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>D</v>
+      </c>
+      <c r="F5">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K5" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C6" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D6" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E6" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F6" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G6" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K6" s="10" t="e">
+      <c r="B6" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C6">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D6" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v xml:space="preserve">na ra na na </v>
+      </c>
+      <c r="E6" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>E</v>
+      </c>
+      <c r="F6">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C7" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D7" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E7" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F7" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G7" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K7" s="10" t="e">
+      <c r="B7" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C7">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D7" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>every day</v>
+      </c>
+      <c r="E7" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>C</v>
+      </c>
+      <c r="F7">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C8" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D8" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E8" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F8" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G8" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K8" s="10" t="e">
+      <c r="B8" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C8">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D8" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v xml:space="preserve">Its like my ipod </v>
+      </c>
+      <c r="E8" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>G</v>
+      </c>
+      <c r="F8">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C9" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D9" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E9" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F9" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G9" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K9" s="10" t="e">
+      <c r="B9" t="str">
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>Replay</v>
+      </c>
+      <c r="C9">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="D9" t="str">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>stuck-on replay</v>
+      </c>
+      <c r="E9" t="str">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>D</v>
+      </c>
+      <c r="F9">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="7">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
-        <v>#NUM!</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C10" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D10" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E10" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F10" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G10" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K10" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K10" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C11" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D11" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E11" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F11" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G11" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K11" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K11" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C12" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D12" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E12" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F12" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G12" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K12" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K12" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C13" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D13" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E13" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F13" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G13" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K13" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K13" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C14" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D14" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E14" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F14" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G14" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K14" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K14" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C15" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D15" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E15" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F15" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G15" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K15" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K15" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C16" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D16" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E16" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F16" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G16" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K16" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K16" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C17" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D17" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E17" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F17" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G17" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K17" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K17" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="C18" t="e">
-        <f>INDEX(CANCIONES!$C$5:$C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="D18" t="e">
-        <f>INDEX(CANCIONES!$D$5:$D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="E18" t="e">
-        <f>INDEX(CANCIONES!$E$5:$E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="F18" t="e">
-        <f>INDEX(CANCIONES!$F$5:$F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
       <c r="G18" t="e">
-        <f>INDEX(CANCIONES!$G$5:$G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K18" s="10" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K18" s="7" t="e">
         <f>SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C19" t="e">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D19" t="e">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E19" t="e">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F19" t="e">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G19" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C20" t="e">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D20" t="e">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E20" t="e">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F20" t="e">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G20" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C21" t="e">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D21" t="e">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E21" t="e">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F21" t="e">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G21" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="e">
-        <f>INDEX(CANCIONES!$B$5:$B$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <f>INDEX(CANCIONES!C$5:C$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C22" t="e">
+        <f>INDEX(CANCIONES!D$5:D$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D22" t="e">
+        <f>INDEX(CANCIONES!E$5:E$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E22" t="e">
+        <f>INDEX(CANCIONES!F$5:F$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F22" t="e">
+        <f>INDEX(CANCIONES!G$5:G$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G22" t="e">
+        <f>INDEX(CANCIONES!H$5:H$100,SMALL('OPERACIONES DE FORMULAS'!$D$5:$D$35,ROW()-1)-4)</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -1650,362 +1756,594 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF2396F-2B00-4C99-BED7-890F3FD75333}">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="D4:D61"/>
+  <dimension ref="D4:G61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="14" t="s">
+    <row r="4" spans="4:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D5" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D7" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D8" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D9" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D10" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D11" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D12" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="G4" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>5</v>
+      </c>
+      <c r="G5" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A5),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v>Replay</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>6</v>
+      </c>
+      <c r="G6" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A6),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>7</v>
+      </c>
+      <c r="G7" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A7),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>8</v>
+      </c>
+      <c r="G8" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A8),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>9</v>
+      </c>
+      <c r="G9" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A9),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>10</v>
+      </c>
+      <c r="G10" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A10),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>11</v>
+      </c>
+      <c r="G11" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A11),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>12</v>
+      </c>
+      <c r="G12" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A12),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G13" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A13),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G14" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A14),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G15" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A15),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D16" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G16" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A16),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G17" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A17),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A18),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A19),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G20" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A20),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G21" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A21),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G22" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A22),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G23" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A23),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G24" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A24),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G25" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A25),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G26" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A26),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G27" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A27),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G28" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A28),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G29" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A29),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G30" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A30),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G31" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A31),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G32" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A32),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G33" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A33),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G34" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A34),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G35" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A35),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A36),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G37" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A37),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G38" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A38),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D39" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G39" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A39),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G40" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A40),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D41" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G41" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A41),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D42" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G42" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A42),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D43" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G43" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A43),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D44" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G44" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A44),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D45" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G45" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A45),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D46" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G46" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A46),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D47" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G47" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A47),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D48" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G48" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A48),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G49" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A49),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D50" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G50" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A50),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D51" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G51" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A51),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D52" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G52" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A52),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D53" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G53" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A53),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D54" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G54" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A54),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D55" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G55" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A55),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D56" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G56" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A56),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D57" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G57" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A57),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D58" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G58" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A58),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D59" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G59" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A59),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D60" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G60" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A60),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D61" t="b">
-        <f>IF(CANCIONES!$B$5:$B$200=Index!$C$2,ROW())</f>
-        <v>0</v>
+        <f>IF(CANCIONES!$C$5:$C$200=Index!$C$2,ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="G61" t="str">
+        <f>IFERROR(INDEX(CANCIONES!$C$5:$C$13,MATCH(ROWS(CANCIONES!$A$5:A61),CANCIONES!$A$5:$A$13,0)),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2016,14 +2354,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2CD92-9487-4DC1-8D1C-E88C0F5EF3CB}">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A2:L12"/>
+  <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="50.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
@@ -2052,229 +2391,244 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="19">
         <f>IF(B5=1,COUNTIF($B$5:B5,1),"")</f>
         <v>1</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="19">
         <f>--ISNUMBER(IFERROR(SEARCH(Index!$C$2,C5,1),""))</f>
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="7">
         <v>1</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <v>1</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>4</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>3</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>4</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="7">
         <v>3</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>4</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="7">
         <v>3</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>4</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="7">
         <v>4</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>4</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="7">
         <v>4</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="str">
+        <f>IF(B13=1,COUNTIF($B$5:B13,1),"")</f>
+        <v/>
+      </c>
+      <c r="B13" s="19">
+        <f>--ISNUMBER(IFERROR(SEARCH(Index!$C$2,C13,1),""))</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2307,18 +2661,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="7">
         <v>13</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
@@ -2340,10 +2694,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="7">
         <v>14</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I3" s="1" t="b">
@@ -2356,10 +2710,10 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="7">
         <v>13</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="1">
@@ -2372,10 +2726,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="7">
         <v>14</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I5" s="1" t="b">
@@ -2388,10 +2742,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="7">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>34</v>
       </c>
       <c r="I6" s="1" t="b">
@@ -2404,10 +2758,10 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="7">
         <v>14</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I7" s="1" t="b">
@@ -2420,10 +2774,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="7">
         <v>13</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="1">
@@ -2436,10 +2790,10 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="7">
         <v>12</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I9" s="1" t="b">
@@ -2452,10 +2806,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>14</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="1" t="b">

</xml_diff>